<commit_message>
16.03.2021 21:23 Data provider hot-fix
</commit_message>
<xml_diff>
--- a/src/main/resources/Dane.xlsx
+++ b/src/main/resources/Dane.xlsx
@@ -184,15 +184,16 @@
   </sheetPr>
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G:G"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
19.03.2021 First test report
</commit_message>
<xml_diff>
--- a/src/main/resources/Dane.xlsx
+++ b/src/main/resources/Dane.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t xml:space="preserve">Miasto</t>
   </si>
@@ -182,13 +182,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.97"/>
@@ -266,6 +266,35 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>